<commit_message>
Pop removed, error in  member payment resolved
</commit_message>
<xml_diff>
--- a/TestResources/TestCaseSheet.xlsx
+++ b/TestResources/TestCaseSheet.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -426,7 +426,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Account Type change from hash map to variable in Account balance pageobjects
</commit_message>
<xml_diff>
--- a/TestResources/TestCaseSheet.xlsx
+++ b/TestResources/TestCaseSheet.xlsx
@@ -426,7 +426,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,7 +462,7 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -476,7 +476,7 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
latest mohit with bug fixes 14/9/17
</commit_message>
<xml_diff>
--- a/TestResources/TestCaseSheet.xlsx
+++ b/TestResources/TestCaseSheet.xlsx
@@ -56,7 +56,7 @@
     <t>MEM005,MEM006,TXN002</t>
   </si>
   <si>
-    <t>,MEM004,MEM009,ACC013,MSG001</t>
+    <t>MEM004,MEM009,ACC013,MSG001</t>
   </si>
 </sst>
 </file>
@@ -433,7 +433,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>